<commit_message>
add N2W childcare needs
</commit_message>
<xml_diff>
--- a/CNA_Survey_Data.xlsx
+++ b/CNA_Survey_Data.xlsx
@@ -11,19 +11,20 @@
     <sheet name="Military Service" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Children living in home" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Single Parent" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Primary Language" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Employment Status" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Public Benefits" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Housing" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Transportation needs" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Incarceration" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Health" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Childcare Needs" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Primary Language" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Employment Status" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Public Benefits" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Housing" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Transportation needs" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Incarceration" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Health" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t xml:space="preserve">survey</t>
   </si>
@@ -203,6 +204,30 @@
   </si>
   <si>
     <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Childcare needs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No, I do not need childcare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No-I do not need help paying for childcare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes-I need after-school or summer care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes-I need help getting childcare for my young children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes-I need help getting infant care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes-I need help paying for after-school and/or summer care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes-I need help paying for childcare</t>
   </si>
   <si>
     <t xml:space="preserve">Primary Language</t>
@@ -2323,19 +2348,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" t="e">
-        <v>#N/A</v>
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
       </c>
       <c r="D2" t="n">
-        <v>149</v>
+        <v>300</v>
       </c>
       <c r="E2" t="n">
         <v>441</v>
       </c>
       <c r="F2" t="n">
-        <v>33.79</v>
+        <v>68.03</v>
       </c>
     </row>
     <row r="3">
@@ -2343,19 +2368,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D3" t="n">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="E3" t="n">
         <v>441</v>
       </c>
       <c r="F3" t="n">
-        <v>27.21</v>
+        <v>25.17</v>
       </c>
     </row>
     <row r="4">
@@ -2363,39 +2388,39 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="C4" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D4" t="n">
-        <v>104</v>
+        <v>30</v>
       </c>
       <c r="E4" t="n">
         <v>441</v>
       </c>
       <c r="F4" t="n">
-        <v>23.58</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="D5" t="n">
-        <v>68</v>
+        <v>1123</v>
       </c>
       <c r="E5" t="n">
-        <v>441</v>
+        <v>1422</v>
       </c>
       <c r="F5" t="n">
-        <v>15.42</v>
+        <v>78.97</v>
       </c>
     </row>
     <row r="6">
@@ -2403,19 +2428,19 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D6" t="n">
-        <v>459</v>
+        <v>188</v>
       </c>
       <c r="E6" t="n">
         <v>1422</v>
       </c>
       <c r="F6" t="n">
-        <v>32.28</v>
+        <v>13.22</v>
       </c>
     </row>
     <row r="7">
@@ -2423,19 +2448,19 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D7" t="n">
-        <v>138</v>
+        <v>92</v>
       </c>
       <c r="E7" t="n">
         <v>1422</v>
       </c>
       <c r="F7" t="n">
-        <v>9.7</v>
+        <v>6.47</v>
       </c>
     </row>
     <row r="8">
@@ -2443,79 +2468,279 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="C8" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D8" t="n">
-        <v>169</v>
+        <v>19</v>
       </c>
       <c r="E8" t="n">
         <v>1422</v>
       </c>
       <c r="F8" t="n">
-        <v>11.88</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
         <v>81</v>
       </c>
       <c r="D9" t="n">
-        <v>239</v>
+        <v>1423</v>
       </c>
       <c r="E9" t="n">
-        <v>1422</v>
+        <v>1863</v>
       </c>
       <c r="F9" t="n">
-        <v>16.81</v>
+        <v>76.38</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="D10" t="n">
-        <v>747</v>
+        <v>203</v>
       </c>
       <c r="E10" t="n">
-        <v>1422</v>
+        <v>1863</v>
       </c>
       <c r="F10" t="n">
-        <v>52.53</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" t="e">
+        <v>80</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="n">
+        <v>188</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1863</v>
+      </c>
+      <c r="F11" t="n">
+        <v>10.09</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D11" t="n">
-        <v>23</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1422</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1.62</v>
+      <c r="D12" t="n">
+        <v>49</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1863</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2.63</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D13" t="n">
+        <v>176</v>
+      </c>
+      <c r="E13" t="n">
+        <v>441</v>
+      </c>
+      <c r="F13" t="n">
+        <v>39.91</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" t="n">
+        <v>137</v>
+      </c>
+      <c r="E14" t="n">
+        <v>441</v>
+      </c>
+      <c r="F14" t="n">
+        <v>31.07</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="n">
+        <v>128</v>
+      </c>
+      <c r="E15" t="n">
+        <v>441</v>
+      </c>
+      <c r="F15" t="n">
+        <v>29.02</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1140</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F16" t="n">
+        <v>80.17</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" t="n">
+        <v>264</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F17" t="n">
+        <v>18.57</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D18" t="n">
+        <v>18</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1268</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1863</v>
+      </c>
+      <c r="F19" t="n">
+        <v>68.06</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="n">
+        <v>401</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1863</v>
+      </c>
+      <c r="F20" t="n">
+        <v>21.52</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D21" t="n">
+        <v>194</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1863</v>
+      </c>
+      <c r="F21" t="n">
+        <v>10.41</v>
       </c>
     </row>
   </sheetData>
@@ -2557,19 +2782,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" t="s">
-        <v>59</v>
+        <v>85</v>
+      </c>
+      <c r="C2" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D2" t="n">
-        <v>266</v>
+        <v>149</v>
       </c>
       <c r="E2" t="n">
         <v>441</v>
       </c>
       <c r="F2" t="n">
-        <v>60.32</v>
+        <v>33.79</v>
       </c>
     </row>
     <row r="3">
@@ -2577,19 +2802,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D3" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E3" t="n">
         <v>441</v>
       </c>
       <c r="F3" t="n">
-        <v>31.75</v>
+        <v>27.21</v>
       </c>
     </row>
     <row r="4">
@@ -2597,39 +2822,39 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" t="e">
-        <v>#N/A</v>
+        <v>85</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
       </c>
       <c r="D4" t="n">
-        <v>35</v>
+        <v>104</v>
       </c>
       <c r="E4" t="n">
         <v>441</v>
       </c>
       <c r="F4" t="n">
-        <v>7.94</v>
+        <v>23.58</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D5" t="n">
-        <v>1300</v>
+        <v>68</v>
       </c>
       <c r="E5" t="n">
-        <v>1422</v>
+        <v>441</v>
       </c>
       <c r="F5" t="n">
-        <v>91.42</v>
+        <v>15.42</v>
       </c>
     </row>
     <row r="6">
@@ -2637,19 +2862,19 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="D6" t="n">
-        <v>101</v>
+        <v>459</v>
       </c>
       <c r="E6" t="n">
         <v>1422</v>
       </c>
       <c r="F6" t="n">
-        <v>7.1</v>
+        <v>32.28</v>
       </c>
     </row>
     <row r="7">
@@ -2657,79 +2882,99 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" t="e">
-        <v>#N/A</v>
+        <v>85</v>
+      </c>
+      <c r="C7" t="s">
+        <v>86</v>
       </c>
       <c r="D7" t="n">
-        <v>21</v>
+        <v>138</v>
       </c>
       <c r="E7" t="n">
         <v>1422</v>
       </c>
       <c r="F7" t="n">
-        <v>1.48</v>
+        <v>9.7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="D8" t="n">
-        <v>1566</v>
+        <v>169</v>
       </c>
       <c r="E8" t="n">
-        <v>1863</v>
+        <v>1422</v>
       </c>
       <c r="F8" t="n">
-        <v>84.06</v>
+        <v>11.88</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="D9" t="n">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E9" t="n">
-        <v>1863</v>
+        <v>1422</v>
       </c>
       <c r="F9" t="n">
-        <v>12.94</v>
+        <v>16.81</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" t="e">
+        <v>85</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="n">
+        <v>747</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F10" t="n">
+        <v>52.53</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" t="e">
         <v>#N/A</v>
       </c>
-      <c r="D10" t="n">
-        <v>56</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1863</v>
-      </c>
-      <c r="F10" t="n">
-        <v>3.01</v>
+      <c r="D11" t="n">
+        <v>23</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.62</v>
       </c>
     </row>
   </sheetData>
@@ -2748,6 +2993,220 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="n">
+        <v>266</v>
+      </c>
+      <c r="E2" t="n">
+        <v>441</v>
+      </c>
+      <c r="F2" t="n">
+        <v>60.32</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="n">
+        <v>140</v>
+      </c>
+      <c r="E3" t="n">
+        <v>441</v>
+      </c>
+      <c r="F3" t="n">
+        <v>31.75</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D4" t="n">
+        <v>35</v>
+      </c>
+      <c r="E4" t="n">
+        <v>441</v>
+      </c>
+      <c r="F4" t="n">
+        <v>7.94</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F5" t="n">
+        <v>91.42</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="n">
+        <v>101</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F6" t="n">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D7" t="n">
+        <v>21</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1566</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1863</v>
+      </c>
+      <c r="F8" t="n">
+        <v>84.06</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" t="n">
+        <v>241</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1863</v>
+      </c>
+      <c r="F9" t="n">
+        <v>12.94</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="D10" t="n">
+        <v>56</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1863</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3.01</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
@@ -2768,7 +3227,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B2" t="n">
         <v>130</v>
@@ -2780,7 +3239,7 @@
         <v>9.14</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
@@ -2788,7 +3247,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B3" t="n">
         <v>97</v>
@@ -2800,7 +3259,7 @@
         <v>6.82</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -2808,7 +3267,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B4" t="n">
         <v>114</v>
@@ -2820,7 +3279,7 @@
         <v>8.02</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -2828,7 +3287,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B5" t="n">
         <v>95</v>
@@ -2840,7 +3299,7 @@
         <v>6.68</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
@@ -2848,7 +3307,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B6" t="n">
         <v>28</v>
@@ -2860,7 +3319,7 @@
         <v>1.97</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
@@ -2880,7 +3339,7 @@
         <v>77.99</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
@@ -2888,7 +3347,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B8" t="n">
         <v>15</v>
@@ -2900,7 +3359,7 @@
         <v>1.05</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
@@ -4258,7 +4717,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>60</v>
@@ -4267,18 +4726,18 @@
         <v>61</v>
       </c>
       <c r="D2" t="n">
-        <v>1016</v>
+        <v>188</v>
       </c>
       <c r="E2" t="n">
-        <v>1422</v>
+        <v>441</v>
       </c>
       <c r="F2" t="n">
-        <v>71.45</v>
+        <v>42.63</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>60</v>
@@ -4287,173 +4746,113 @@
         <v>62</v>
       </c>
       <c r="D3" t="n">
-        <v>210</v>
+        <v>58</v>
       </c>
       <c r="E3" t="n">
-        <v>1422</v>
+        <v>441</v>
       </c>
       <c r="F3" t="n">
-        <v>14.77</v>
+        <v>13.15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="D4" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" t="n">
-        <v>1422</v>
+        <v>441</v>
       </c>
       <c r="F4" t="n">
-        <v>4.01</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D5" t="n">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="E5" t="n">
-        <v>1422</v>
+        <v>441</v>
       </c>
       <c r="F5" t="n">
-        <v>2.67</v>
+        <v>6.35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D6" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E6" t="n">
-        <v>1422</v>
+        <v>441</v>
       </c>
       <c r="F6" t="n">
-        <v>2.6</v>
+        <v>7.71</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D7" t="n">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E7" t="n">
-        <v>1422</v>
+        <v>441</v>
       </c>
       <c r="F7" t="n">
-        <v>2.32</v>
+        <v>9.98</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>60</v>
       </c>
-      <c r="C8" t="e">
-        <v>#N/A</v>
+      <c r="C8" t="s">
+        <v>67</v>
       </c>
       <c r="D8" t="n">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="E8" t="n">
-        <v>1422</v>
+        <v>441</v>
       </c>
       <c r="F8" t="n">
-        <v>1.13</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" t="n">
-        <v>8</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1422</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.56</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" t="n">
-        <v>6</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1422</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1422</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.07</v>
+        <v>10.43</v>
       </c>
     </row>
   </sheetData>
@@ -4492,62 +4891,62 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
       <c r="D2" t="n">
-        <v>237</v>
+        <v>1016</v>
       </c>
       <c r="E2" t="n">
-        <v>441</v>
+        <v>1422</v>
       </c>
       <c r="F2" t="n">
-        <v>53.74</v>
+        <v>71.45</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="D3" t="n">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="E3" t="n">
-        <v>441</v>
+        <v>1422</v>
       </c>
       <c r="F3" t="n">
-        <v>41.5</v>
+        <v>14.77</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" t="e">
-        <v>#N/A</v>
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
       </c>
       <c r="D4" t="n">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="E4" t="n">
-        <v>441</v>
+        <v>1422</v>
       </c>
       <c r="F4" t="n">
-        <v>4.76</v>
+        <v>4.01</v>
       </c>
     </row>
     <row r="5">
@@ -4555,19 +4954,19 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D5" t="n">
-        <v>989</v>
+        <v>38</v>
       </c>
       <c r="E5" t="n">
         <v>1422</v>
       </c>
       <c r="F5" t="n">
-        <v>69.55</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="6">
@@ -4575,19 +4974,19 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D6" t="n">
-        <v>423</v>
+        <v>37</v>
       </c>
       <c r="E6" t="n">
         <v>1422</v>
       </c>
       <c r="F6" t="n">
-        <v>29.75</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="7">
@@ -4595,79 +4994,99 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" t="e">
-        <v>#N/A</v>
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E7" t="n">
         <v>1422</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7</v>
+        <v>2.32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="C8" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D8" t="n">
-        <v>1226</v>
+        <v>16</v>
       </c>
       <c r="E8" t="n">
-        <v>1863</v>
+        <v>1422</v>
       </c>
       <c r="F8" t="n">
-        <v>65.81</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D9" t="n">
-        <v>606</v>
+        <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>1863</v>
+        <v>1422</v>
       </c>
       <c r="F9" t="n">
-        <v>32.53</v>
+        <v>0.56</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" t="e">
-        <v>#N/A</v>
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
       </c>
       <c r="D10" t="n">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E10" t="n">
-        <v>1863</v>
+        <v>1422</v>
       </c>
       <c r="F10" t="n">
-        <v>1.66</v>
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1422</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.07</v>
       </c>
     </row>
   </sheetData>
@@ -4709,19 +5128,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D2" t="n">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="E2" t="n">
         <v>441</v>
       </c>
       <c r="F2" t="n">
-        <v>51.02</v>
+        <v>53.74</v>
       </c>
     </row>
     <row r="3">
@@ -4729,19 +5148,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
         <v>59</v>
       </c>
       <c r="D3" t="n">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E3" t="n">
         <v>441</v>
       </c>
       <c r="F3" t="n">
-        <v>43.08</v>
+        <v>41.5</v>
       </c>
     </row>
     <row r="4">
@@ -4749,19 +5168,19 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" t="e">
         <v>#N/A</v>
       </c>
       <c r="D4" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E4" t="n">
         <v>441</v>
       </c>
       <c r="F4" t="n">
-        <v>5.9</v>
+        <v>4.76</v>
       </c>
     </row>
     <row r="5">
@@ -4769,19 +5188,19 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D5" t="n">
-        <v>857</v>
+        <v>989</v>
       </c>
       <c r="E5" t="n">
         <v>1422</v>
       </c>
       <c r="F5" t="n">
-        <v>60.27</v>
+        <v>69.55</v>
       </c>
     </row>
     <row r="6">
@@ -4789,19 +5208,19 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
         <v>59</v>
       </c>
       <c r="D6" t="n">
-        <v>549</v>
+        <v>423</v>
       </c>
       <c r="E6" t="n">
         <v>1422</v>
       </c>
       <c r="F6" t="n">
-        <v>38.61</v>
+        <v>29.75</v>
       </c>
     </row>
     <row r="7">
@@ -4809,19 +5228,19 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C7" t="e">
         <v>#N/A</v>
       </c>
       <c r="D7" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E7" t="n">
         <v>1422</v>
       </c>
       <c r="F7" t="n">
-        <v>1.13</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="8">
@@ -4829,19 +5248,19 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D8" t="n">
-        <v>1082</v>
+        <v>1226</v>
       </c>
       <c r="E8" t="n">
         <v>1863</v>
       </c>
       <c r="F8" t="n">
-        <v>58.08</v>
+        <v>65.81</v>
       </c>
     </row>
     <row r="9">
@@ -4849,19 +5268,19 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
         <v>59</v>
       </c>
       <c r="D9" t="n">
-        <v>739</v>
+        <v>606</v>
       </c>
       <c r="E9" t="n">
         <v>1863</v>
       </c>
       <c r="F9" t="n">
-        <v>39.67</v>
+        <v>32.53</v>
       </c>
     </row>
     <row r="10">
@@ -4869,19 +5288,19 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C10" t="e">
         <v>#N/A</v>
       </c>
       <c r="D10" t="n">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E10" t="n">
         <v>1863</v>
       </c>
       <c r="F10" t="n">
-        <v>2.25</v>
+        <v>1.66</v>
       </c>
     </row>
   </sheetData>
@@ -4923,19 +5342,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D2" t="n">
-        <v>300</v>
+        <v>225</v>
       </c>
       <c r="E2" t="n">
         <v>441</v>
       </c>
       <c r="F2" t="n">
-        <v>68.03</v>
+        <v>51.02</v>
       </c>
     </row>
     <row r="3">
@@ -4943,19 +5362,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="D3" t="n">
-        <v>111</v>
+        <v>190</v>
       </c>
       <c r="E3" t="n">
         <v>441</v>
       </c>
       <c r="F3" t="n">
-        <v>25.17</v>
+        <v>43.08</v>
       </c>
     </row>
     <row r="4">
@@ -4963,19 +5382,19 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C4" t="e">
         <v>#N/A</v>
       </c>
       <c r="D4" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E4" t="n">
         <v>441</v>
       </c>
       <c r="F4" t="n">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="5">
@@ -4983,19 +5402,19 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D5" t="n">
-        <v>1123</v>
+        <v>857</v>
       </c>
       <c r="E5" t="n">
         <v>1422</v>
       </c>
       <c r="F5" t="n">
-        <v>78.97</v>
+        <v>60.27</v>
       </c>
     </row>
     <row r="6">
@@ -5003,19 +5422,19 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D6" t="n">
-        <v>188</v>
+        <v>549</v>
       </c>
       <c r="E6" t="n">
         <v>1422</v>
       </c>
       <c r="F6" t="n">
-        <v>13.22</v>
+        <v>38.61</v>
       </c>
     </row>
     <row r="7">
@@ -5023,39 +5442,39 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" t="s">
-        <v>74</v>
+        <v>79</v>
+      </c>
+      <c r="C7" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D7" t="n">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="E7" t="n">
         <v>1422</v>
       </c>
       <c r="F7" t="n">
-        <v>6.47</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" t="e">
-        <v>#N/A</v>
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
       </c>
       <c r="D8" t="n">
-        <v>19</v>
+        <v>1082</v>
       </c>
       <c r="E8" t="n">
-        <v>1422</v>
+        <v>1863</v>
       </c>
       <c r="F8" t="n">
-        <v>1.34</v>
+        <v>58.08</v>
       </c>
     </row>
     <row r="9">
@@ -5063,19 +5482,19 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D9" t="n">
-        <v>1423</v>
+        <v>739</v>
       </c>
       <c r="E9" t="n">
         <v>1863</v>
       </c>
       <c r="F9" t="n">
-        <v>76.38</v>
+        <v>39.67</v>
       </c>
     </row>
     <row r="10">
@@ -5083,239 +5502,19 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" t="s">
-        <v>74</v>
+        <v>79</v>
+      </c>
+      <c r="C10" t="e">
+        <v>#N/A</v>
       </c>
       <c r="D10" t="n">
-        <v>203</v>
+        <v>42</v>
       </c>
       <c r="E10" t="n">
         <v>1863</v>
       </c>
       <c r="F10" t="n">
-        <v>10.9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" t="n">
-        <v>188</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1863</v>
-      </c>
-      <c r="F11" t="n">
-        <v>10.09</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D12" t="n">
-        <v>49</v>
-      </c>
-      <c r="E12" t="n">
-        <v>1863</v>
-      </c>
-      <c r="F12" t="n">
-        <v>2.63</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D13" t="n">
-        <v>176</v>
-      </c>
-      <c r="E13" t="n">
-        <v>441</v>
-      </c>
-      <c r="F13" t="n">
-        <v>39.91</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" t="n">
-        <v>137</v>
-      </c>
-      <c r="E14" t="n">
-        <v>441</v>
-      </c>
-      <c r="F14" t="n">
-        <v>31.07</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" t="n">
-        <v>128</v>
-      </c>
-      <c r="E15" t="n">
-        <v>441</v>
-      </c>
-      <c r="F15" t="n">
-        <v>29.02</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" t="n">
-        <v>1140</v>
-      </c>
-      <c r="E16" t="n">
-        <v>1422</v>
-      </c>
-      <c r="F16" t="n">
-        <v>80.17</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" t="n">
-        <v>264</v>
-      </c>
-      <c r="E17" t="n">
-        <v>1422</v>
-      </c>
-      <c r="F17" t="n">
-        <v>18.57</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D18" t="n">
-        <v>18</v>
-      </c>
-      <c r="E18" t="n">
-        <v>1422</v>
-      </c>
-      <c r="F18" t="n">
-        <v>1.27</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1268</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1863</v>
-      </c>
-      <c r="F19" t="n">
-        <v>68.06</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" t="n">
-        <v>401</v>
-      </c>
-      <c r="E20" t="n">
-        <v>1863</v>
-      </c>
-      <c r="F20" t="n">
-        <v>21.52</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C21" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="D21" t="n">
-        <v>194</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1863</v>
-      </c>
-      <c r="F21" t="n">
-        <v>10.41</v>
+        <v>2.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>